<commit_message>
Add Manufacturer and Manufacturer Product Number columns to BOM files
</commit_message>
<xml_diff>
--- a/6button-MegaDrive-controller-PCB-DigiKey-BOM.xlsx
+++ b/6button-MegaDrive-controller-PCB-DigiKey-BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t xml:space="preserve">Digi-Key Part Number</t>
   </si>
@@ -34,6 +34,12 @@
     <t xml:space="preserve">Value</t>
   </si>
   <si>
+    <t xml:space="preserve">Manufacturer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacturer Product Number</t>
+  </si>
+  <si>
     <t xml:space="preserve">Description</t>
   </si>
   <si>
@@ -49,6 +55,12 @@
     <t xml:space="preserve">0.1u</t>
   </si>
   <si>
+    <t xml:space="preserve">KYOCERA AVX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KGM21NR71H104KT</t>
+  </si>
+  <si>
     <t xml:space="preserve">CAP CER 0.1UF 50V X7R 0805 – Only 3 needed but cheaper to buy 10 than 3</t>
   </si>
   <si>
@@ -64,6 +76,12 @@
     <t xml:space="preserve">CONN HEADER VERT 14POS 2.54MM</t>
   </si>
   <si>
+    <t xml:space="preserve">TE Connectivity AMP Connectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">826632-7</t>
+  </si>
+  <si>
     <t xml:space="preserve">Connector Header Through Hole 14 position 0.100" (2.54mm)</t>
   </si>
   <si>
@@ -76,6 +94,12 @@
     <t xml:space="preserve">CONN HEADER VERT 9POS 2.54MM</t>
   </si>
   <si>
+    <t xml:space="preserve">Adam Tech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH1-09-UA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Connector Header Through Hole 9 position 0.100" (2.54mm)</t>
   </si>
   <si>
@@ -88,6 +112,9 @@
     <t xml:space="preserve">CONN HEADER VERT 6POS 2.54MM</t>
   </si>
   <si>
+    <t xml:space="preserve">BHR-06-VUA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Connector Header Through Hole 6 position 0.100" (2.54mm)</t>
   </si>
   <si>
@@ -100,6 +127,12 @@
     <t xml:space="preserve">75k</t>
   </si>
   <si>
+    <t xml:space="preserve">TE Connectivity Passive Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPF0805B75KE1</t>
+  </si>
+  <si>
     <t xml:space="preserve">75 kOhms ±0.1% 0.1W, 1/10W Chip Resistor 0805 (2012 Metric) Thin Film</t>
   </si>
   <si>
@@ -112,6 +145,12 @@
     <t xml:space="preserve">74HC257</t>
   </si>
   <si>
+    <t xml:space="preserve">Texas Instruments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD74HC257M96</t>
+  </si>
+  <si>
     <t xml:space="preserve">Multiplexer 4 x 2:1 16-SOIC</t>
   </si>
   <si>
@@ -125,6 +164,9 @@
   </si>
   <si>
     <t xml:space="preserve">ATTINY404-SSNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microchip Technology</t>
   </si>
   <si>
     <t xml:space="preserve">AVR tinyAVR™ 0, Functional Safety (FuSa) Microcontroller IC 8-Bit 20MHz 4KB (4K x 8) FLASH 14-SOIC</t>
@@ -140,7 +182,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -176,6 +218,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -220,7 +267,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -234,6 +281,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -254,7 +305,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -266,8 +317,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="37.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="87.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="55.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="28.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="27.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="87.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="55.68"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -289,149 +342,197 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>